<commit_message>
revisão programação e scraping
</commit_message>
<xml_diff>
--- a/Quote_History_BB/#LISTA_FUNDOS.xlsx
+++ b/Quote_History_BB/#LISTA_FUNDOS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GITHUB\Trend_Fundos_BB\Quote_History_BB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D053055-FBEB-47B8-A38F-72BD8CF51282}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72AD0291-0CD8-4AE7-B576-CC21E885BC68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="15264" yWindow="0" windowWidth="15552" windowHeight="18576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="292">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="303">
   <si>
     <t>BB Ações Setor Financeiro</t>
   </si>
@@ -738,9 +738,6 @@
     <t>BB Ações Games BDR Nível I</t>
   </si>
   <si>
-    <t>https://bb.com.br/uci/fundos.html?gfi=1846&amp;tipo=pf</t>
-  </si>
-  <si>
     <t>Compor uma carteira de ativos financeiros direcionada, preferencialmente, por ativos de renda variável que reflitam a estratégia de SuperDividends, gerida pela Global X</t>
   </si>
   <si>
@@ -904,6 +901,42 @@
   </si>
   <si>
     <t>06.349.816/0001-01</t>
+  </si>
+  <si>
+    <t>https://bb.com.br/uci/informe-mensal.html?gfi=25&amp;tipo=pf</t>
+  </si>
+  <si>
+    <t>01.578.474/0001-88</t>
+  </si>
+  <si>
+    <t xml:space="preserve">O BB Ações Tecnologia BDR Nível I é um fundo temático, que investe em companhias brasileira e estrangeiras dos setores de tecnologia. Tais investimentos ocorrem em empresas dos mais diversos setores econômicos, desde que estas sejam intensivas em tecnologia. </t>
+  </si>
+  <si>
+    <t>O BB Ações US Biotech BDR Nível I é um fundo temático com portfólio de empresas globais, inovadoras pertencentes aos setores de biotecnologia, farmacêutico ou do setor da saúde que possuem elevados investimentos em pesquisa desenvolvimento. O fundo possui proteção cambial, ou seja, a rentabilidade é decorrente do retorno das ações selecionadas para compor a carteira, não sofrendo o impacto do câmbio.</t>
+  </si>
+  <si>
+    <t>38.110.562/0001-60</t>
+  </si>
+  <si>
+    <t>https://bb.com.br/uci/informe-mensal.html?gfi=1763&amp;tipo=pf</t>
+  </si>
+  <si>
+    <t>https://bb.com.br/uci/informe-mensal.html?gfi=504&amp;tipo=pf</t>
+  </si>
+  <si>
+    <t>Este fundo busca agregar rentabilidade aos recursos através de operações que acompanhem a variação do Euro. Para isso, investe em cotas de fundos de investimento, cuja carteira seja composta por: títulos públicos, ativos financeiros negociados no exterior, operações compromissadas lastreadas em títulos públicos federais, títulos de emissão privada, etc.</t>
+  </si>
+  <si>
+    <t>04.305.193/0001-40</t>
+  </si>
+  <si>
+    <t>40.021.803/0001-47</t>
+  </si>
+  <si>
+    <t>https://bb.com.br/uci/informe-mensal.html?gfi=1846</t>
+  </si>
+  <si>
+    <t>08.080.680/0001-02</t>
   </si>
 </sst>
 </file>
@@ -1399,10 +1432,10 @@
   <dimension ref="A1:U55"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C35" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E8" sqref="E8"/>
+      <selection pane="bottomRight" activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1453,7 +1486,7 @@
         <v>222</v>
       </c>
       <c r="H1" s="7" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="I1" s="3" t="s">
         <v>100</v>
@@ -2110,7 +2143,7 @@
       </c>
       <c r="D13" s="16"/>
       <c r="E13" s="17" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="F13" s="17" t="s">
         <v>203</v>
@@ -2157,10 +2190,10 @@
       </c>
       <c r="D14" s="16"/>
       <c r="E14" s="17" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="F14" s="17" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="G14" s="4">
         <v>5</v>
@@ -2204,7 +2237,7 @@
       </c>
       <c r="D15" s="16"/>
       <c r="E15" s="17" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F15" s="17" t="s">
         <v>209</v>
@@ -2580,7 +2613,9 @@
       <c r="B22" s="16" t="s">
         <v>235</v>
       </c>
-      <c r="C22" s="16"/>
+      <c r="C22" s="16" t="s">
+        <v>300</v>
+      </c>
       <c r="D22" s="16"/>
       <c r="E22" s="17"/>
       <c r="F22" s="17"/>
@@ -2595,7 +2630,7 @@
       </c>
       <c r="J22" s="19"/>
       <c r="K22" s="22" t="s">
-        <v>236</v>
+        <v>301</v>
       </c>
       <c r="L22" s="18">
         <v>1</v>
@@ -2622,14 +2657,14 @@
         <v>6</v>
       </c>
       <c r="C23" s="23" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D23" s="23"/>
       <c r="E23" s="19" t="s">
         <v>72</v>
       </c>
       <c r="F23" s="17" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="G23" s="18">
         <v>5</v>
@@ -2642,7 +2677,7 @@
       </c>
       <c r="J23" s="19"/>
       <c r="K23" s="22" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="L23" s="18">
         <v>1</v>
@@ -2677,14 +2712,14 @@
         <v>33</v>
       </c>
       <c r="C24" s="16" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D24" s="16"/>
       <c r="E24" s="17" t="s">
         <v>60</v>
       </c>
       <c r="F24" s="17" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="G24" s="18">
         <v>5</v>
@@ -2697,7 +2732,7 @@
       </c>
       <c r="J24" s="19"/>
       <c r="K24" s="22" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="L24" s="18">
         <v>1</v>
@@ -2732,14 +2767,14 @@
         <v>39</v>
       </c>
       <c r="C25" s="16" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D25" s="16"/>
       <c r="E25" s="17" t="s">
         <v>68</v>
       </c>
       <c r="F25" s="17" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="G25" s="18">
         <v>5</v>
@@ -2752,7 +2787,7 @@
       </c>
       <c r="J25" s="19"/>
       <c r="K25" s="22" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="L25" s="18">
         <v>1</v>
@@ -2787,14 +2822,14 @@
         <v>2</v>
       </c>
       <c r="C26" s="23" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D26" s="23"/>
       <c r="E26" s="19" t="s">
         <v>61</v>
       </c>
       <c r="F26" s="17" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="G26" s="18">
         <v>5</v>
@@ -2807,7 +2842,7 @@
       </c>
       <c r="J26" s="19"/>
       <c r="K26" s="22" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="L26" s="18">
         <v>1</v>
@@ -2840,14 +2875,14 @@
         <v>27</v>
       </c>
       <c r="C27" s="16" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D27" s="16"/>
       <c r="E27" s="17" t="s">
         <v>99</v>
       </c>
       <c r="F27" s="17" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="G27" s="18">
         <v>5</v>
@@ -2860,7 +2895,7 @@
       </c>
       <c r="J27" s="19"/>
       <c r="K27" s="22" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="L27" s="18">
         <v>0</v>
@@ -2893,14 +2928,14 @@
         <v>84</v>
       </c>
       <c r="C28" s="16" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D28" s="16"/>
       <c r="E28" s="17" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="F28" s="17" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="G28" s="18">
         <v>5</v>
@@ -2913,7 +2948,7 @@
       </c>
       <c r="J28" s="19"/>
       <c r="K28" s="22" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="L28" s="18">
         <v>1</v>
@@ -2940,14 +2975,14 @@
         <v>12</v>
       </c>
       <c r="C29" s="23" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D29" s="23"/>
       <c r="E29" s="19" t="s">
         <v>73</v>
       </c>
       <c r="F29" s="17" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="G29" s="18">
         <v>5</v>
@@ -2960,7 +2995,7 @@
       </c>
       <c r="J29" s="19"/>
       <c r="K29" s="22" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="L29" s="18">
         <v>1</v>
@@ -2995,14 +3030,14 @@
         <v>0</v>
       </c>
       <c r="C30" s="23" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D30" s="23"/>
       <c r="E30" s="19" t="s">
         <v>69</v>
       </c>
       <c r="F30" s="17" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="G30" s="18">
         <v>5</v>
@@ -3015,7 +3050,7 @@
       </c>
       <c r="J30" s="19"/>
       <c r="K30" s="22" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="L30" s="18">
         <v>1</v>
@@ -3050,14 +3085,14 @@
         <v>1</v>
       </c>
       <c r="C31" s="23" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D31" s="23"/>
       <c r="E31" s="19" t="s">
         <v>74</v>
       </c>
       <c r="F31" s="17" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="G31" s="18">
         <v>5</v>
@@ -3070,7 +3105,7 @@
       </c>
       <c r="J31" s="19"/>
       <c r="K31" s="22" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="L31" s="18">
         <v>1</v>
@@ -3105,14 +3140,14 @@
         <v>3</v>
       </c>
       <c r="C32" s="23" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="D32" s="23"/>
       <c r="E32" s="19" t="s">
         <v>51</v>
       </c>
       <c r="F32" s="17" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="G32" s="18">
         <v>5</v>
@@ -3127,7 +3162,7 @@
         <v>49</v>
       </c>
       <c r="K32" s="22" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="L32" s="18">
         <v>1</v>
@@ -3164,14 +3199,14 @@
         <v>83</v>
       </c>
       <c r="C33" s="16" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="D33" s="16"/>
       <c r="E33" s="17" t="s">
         <v>96</v>
       </c>
       <c r="F33" s="17" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="G33" s="18">
         <v>5</v>
@@ -3184,7 +3219,7 @@
       </c>
       <c r="J33" s="19"/>
       <c r="K33" s="22" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="L33" s="18">
         <v>1</v>
@@ -3209,29 +3244,45 @@
       </c>
       <c r="U33" s="25"/>
     </row>
-    <row r="34" spans="1:21" s="21" customFormat="1" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:21" s="21" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A34" s="12" t="s">
         <v>152</v>
       </c>
       <c r="B34" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="C34" s="16"/>
+      <c r="C34" s="16" t="s">
+        <v>292</v>
+      </c>
       <c r="D34" s="16"/>
       <c r="E34" s="17" t="s">
         <v>75</v>
       </c>
-      <c r="F34" s="17"/>
-      <c r="G34" s="18"/>
-      <c r="H34" s="16"/>
+      <c r="F34" s="17" t="s">
+        <v>293</v>
+      </c>
+      <c r="G34" s="18">
+        <v>5</v>
+      </c>
+      <c r="H34" s="16" t="s">
+        <v>110</v>
+      </c>
       <c r="I34" s="18" t="s">
         <v>101</v>
       </c>
       <c r="J34" s="19"/>
-      <c r="K34" s="19"/>
-      <c r="L34" s="18"/>
-      <c r="M34" s="18"/>
-      <c r="N34" s="18"/>
+      <c r="K34" s="22" t="s">
+        <v>291</v>
+      </c>
+      <c r="L34" s="18">
+        <v>1</v>
+      </c>
+      <c r="M34" s="18">
+        <v>1</v>
+      </c>
+      <c r="N34" s="18">
+        <v>3</v>
+      </c>
       <c r="O34" s="18"/>
       <c r="P34" s="19"/>
       <c r="Q34" s="19"/>
@@ -3248,35 +3299,45 @@
         <v>21</v>
       </c>
     </row>
-    <row r="35" spans="1:21" s="21" customFormat="1" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:21" s="21" customFormat="1" ht="168" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="12" t="s">
         <v>153</v>
       </c>
       <c r="B35" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="C35" s="16"/>
+      <c r="C35" s="16" t="s">
+        <v>295</v>
+      </c>
       <c r="D35" s="16"/>
       <c r="E35" s="17" t="s">
         <v>76</v>
       </c>
-      <c r="F35" s="17"/>
+      <c r="F35" s="17" t="s">
+        <v>294</v>
+      </c>
       <c r="G35" s="18">
         <v>5</v>
       </c>
-      <c r="H35" s="16"/>
+      <c r="H35" s="16" t="s">
+        <v>110</v>
+      </c>
       <c r="I35" s="18" t="s">
         <v>101</v>
       </c>
       <c r="J35" s="19"/>
-      <c r="K35" s="19"/>
+      <c r="K35" s="22" t="s">
+        <v>296</v>
+      </c>
       <c r="L35" s="18">
         <v>1</v>
       </c>
       <c r="M35" s="18">
         <v>1</v>
       </c>
-      <c r="N35" s="18"/>
+      <c r="N35" s="18">
+        <v>3</v>
+      </c>
       <c r="O35" s="18"/>
       <c r="P35" s="19"/>
       <c r="Q35" s="19"/>
@@ -3350,29 +3411,45 @@
         <v>21</v>
       </c>
     </row>
-    <row r="37" spans="1:21" s="21" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:21" s="21" customFormat="1" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A37" s="12" t="s">
         <v>155</v>
       </c>
       <c r="B37" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="C37" s="23"/>
+      <c r="C37" s="23" t="s">
+        <v>299</v>
+      </c>
       <c r="D37" s="23"/>
       <c r="E37" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="F37" s="17"/>
-      <c r="G37" s="18"/>
-      <c r="H37" s="23"/>
+      <c r="F37" s="17" t="s">
+        <v>298</v>
+      </c>
+      <c r="G37" s="18">
+        <v>5</v>
+      </c>
+      <c r="H37" s="23" t="s">
+        <v>102</v>
+      </c>
       <c r="I37" s="18" t="s">
         <v>105</v>
       </c>
       <c r="J37" s="19"/>
-      <c r="K37" s="19"/>
-      <c r="L37" s="18"/>
-      <c r="M37" s="18"/>
-      <c r="N37" s="18"/>
+      <c r="K37" s="22" t="s">
+        <v>297</v>
+      </c>
+      <c r="L37" s="18">
+        <v>0</v>
+      </c>
+      <c r="M37" s="18">
+        <v>0</v>
+      </c>
+      <c r="N37" s="18">
+        <v>0</v>
+      </c>
       <c r="O37" s="18"/>
       <c r="P37" s="19"/>
       <c r="Q37" s="19"/>
@@ -3680,7 +3757,7 @@
         <v>30</v>
       </c>
       <c r="C47" s="9" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D47" s="9"/>
       <c r="E47" s="13" t="s">
@@ -3700,7 +3777,7 @@
       </c>
       <c r="J47" s="12"/>
       <c r="K47" s="11" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="L47" s="4">
         <v>0</v>
@@ -3772,25 +3849,25 @@
         <v>86</v>
       </c>
       <c r="C49" s="9" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D49" s="9"/>
       <c r="E49" s="13"/>
       <c r="F49" s="13" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="G49" s="4">
         <v>5</v>
       </c>
       <c r="H49" s="9" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="I49" s="18" t="s">
         <v>105</v>
       </c>
       <c r="J49" s="12"/>
       <c r="K49" s="11" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="L49" s="4">
         <v>1</v>
@@ -3817,12 +3894,12 @@
         <v>92</v>
       </c>
       <c r="C50" s="9" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D50" s="9"/>
       <c r="E50" s="13"/>
       <c r="F50" s="13" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="G50" s="4">
         <v>3</v>
@@ -3835,7 +3912,7 @@
       </c>
       <c r="J50" s="12"/>
       <c r="K50" s="11" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="L50" s="4">
         <v>1</v>
@@ -3862,12 +3939,12 @@
         <v>94</v>
       </c>
       <c r="C51" s="9" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D51" s="9"/>
       <c r="E51" s="13"/>
       <c r="F51" s="13" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="G51" s="4">
         <v>3</v>
@@ -3880,7 +3957,7 @@
       </c>
       <c r="J51" s="12"/>
       <c r="K51" s="11" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="L51" s="4">
         <v>1</v>
@@ -3907,14 +3984,14 @@
         <v>22</v>
       </c>
       <c r="C52" s="9" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D52" s="9"/>
       <c r="E52" s="13" t="s">
         <v>22</v>
       </c>
       <c r="F52" s="13" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="G52" s="4">
         <v>2</v>
@@ -3927,7 +4004,7 @@
       </c>
       <c r="J52" s="12"/>
       <c r="K52" s="11" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="L52" s="4">
         <v>0</v>
@@ -3961,7 +4038,9 @@
       <c r="B53" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="C53" s="9"/>
+      <c r="C53" s="9" t="s">
+        <v>302</v>
+      </c>
       <c r="D53" s="9"/>
       <c r="E53" s="13" t="s">
         <v>23</v>
@@ -4001,7 +4080,7 @@
     </row>
     <row r="54" spans="1:21" ht="112.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="12" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B54" s="9" t="s">
         <v>40</v>
@@ -4116,6 +4195,9 @@
     <hyperlink ref="K31" r:id="rId42" xr:uid="{C07B4734-2D5D-46BE-8ECC-DAC1952E914D}"/>
     <hyperlink ref="K32" r:id="rId43" xr:uid="{2C04A4E9-864A-454A-B002-050C5A59B11F}"/>
     <hyperlink ref="K33" r:id="rId44" xr:uid="{0A5D9B41-C2D4-454E-94AD-2B04A2CA403C}"/>
+    <hyperlink ref="K34" r:id="rId45" xr:uid="{2AC42EB6-31A0-4FFB-A07F-EF34FB769A95}"/>
+    <hyperlink ref="K35" r:id="rId46" xr:uid="{33E2673B-1435-4D3A-91A9-85C72E4B2FB9}"/>
+    <hyperlink ref="K37" r:id="rId47" xr:uid="{D3027F1C-7002-4E2F-ACBC-E3356AD1AD51}"/>
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>